<commit_message>
Dirct commit skipping staging area, changed text and excel
</commit_message>
<xml_diff>
--- a/repair.xlsx
+++ b/repair.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>hello</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>change</t>
+  </si>
+  <si>
+    <t>second</t>
   </si>
 </sst>
 </file>
@@ -359,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -380,6 +383,14 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>